<commit_message>
Pareto Coefficients from WID Database
</commit_message>
<xml_diff>
--- a/estimates/taxReform1990.xlsx
+++ b/estimates/taxReform1990.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>estimate</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>https://ideas.repec.org/b/oxp/obooks/9780199286898.html</t>
+  </si>
+  <si>
+    <t>As estimated by downloadParetoCoefficient.R in the taxReform1990 folder</t>
+  </si>
+  <si>
+    <t>pareto_coefficient_1990_wid</t>
   </si>
 </sst>
 </file>
@@ -889,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,6 +972,9 @@
       <c r="G2">
         <v>5.0000000000000001E-4</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
       <c r="K2" t="s">
         <v>14</v>
       </c>
@@ -986,11 +995,31 @@
       <c r="C3">
         <v>0</v>
       </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
       <c r="K3" t="s">
         <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1.9941679999999999</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made sense of all the tax reforms between 2000 and 2005: * Splitted the 2000 Reforms in 3 Reforms:  ** 2001 (53% -> 48.5%)  ** 2004 (48.5% -> 45%)  ** 2005 (45% -> 42%)
</commit_message>
<xml_diff>
--- a/estimates/taxReform1990.xlsx
+++ b/estimates/taxReform1990.xlsx
@@ -81,10 +81,10 @@
     <t>https://ideas.repec.org/b/oxp/obooks/9780199286898.html</t>
   </si>
   <si>
-    <t>As estimated by downloadParetoCoefficient.R in the taxReform1990 folder</t>
-  </si>
-  <si>
     <t>pareto_coefficient_1990_wid</t>
+  </si>
+  <si>
+    <t>Calculated from data by the World Inequality Databse. See downloadParetoCoefficient.R in the taxReform1990 folder for details.</t>
   </si>
 </sst>
 </file>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,9 +1005,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>1.9941679999999999</v>
@@ -1019,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added plot for just the income tax.
</commit_message>
<xml_diff>
--- a/estimates/taxReform1990.xlsx
+++ b/estimates/taxReform1990.xlsx
@@ -69,9 +69,6 @@
     <t>https://ideas.repec.org/p/iaw/iawdip/15.html</t>
   </si>
   <si>
-    <t>Authors report a "error probability" of 0.000. This has to be the p-value. Any p value smaller than 0.0005 rounds to 0.000</t>
-  </si>
-  <si>
     <t>pareto_coefficient_1989</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Calculated from data by the World Inequality Databse. See downloadParetoCoefficient.R in the taxReform1990 folder for details.</t>
+  </si>
+  <si>
+    <t>Authors report a "error probability" of 0.000. This has to be the p-value. Any p value smaller than 0.0005 rounds to 0.000. Selected this specification because Saez et al. (2009) refer to this spec in their survey of empirical ETI estimation. This is a rather high estimate. The paper by Gottfried &amp; Schellhorn (2004) is not that conclusive as results appear to be quite unstable and sensitive to different specifications. But I am not aware of any other literature which analyses explicitely the 1990 reform.</t>
   </si>
 </sst>
 </file>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -982,12 +982,12 @@
         <v>15</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>1.71</v>
@@ -999,15 +999,15 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>1.9941679999999999</v>
@@ -1019,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* updated taxReform1990 to use the same elasticity estimate as the other reforms
</commit_message>
<xml_diff>
--- a/estimates/taxReform1990.xlsx
+++ b/estimates/taxReform1990.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>estimate</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Authors report a "error probability" of 0.000. This has to be the p-value. Any p value smaller than 0.0005 rounds to 0.000. Selected this specification because Saez et al. (2009) refer to this spec in their survey of empirical ETI estimation. This is a rather high estimate. The paper by Gottfried &amp; Schellhorn (2004) is not that conclusive as results appear to be quite unstable and sensitive to different specifications. But I am not aware of any other literature which analyses explicitely the 1990 reform.</t>
+  </si>
+  <si>
+    <t>Doerrenberg et. al. (2015) CESifo Working Paper Table 3</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/ces/ceswps/_5369.html</t>
+  </si>
+  <si>
+    <t>elasticity_of_taxable_income_doerrenberg_2015</t>
   </si>
 </sst>
 </file>
@@ -895,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,6 +1031,26 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="D5">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>